<commit_message>
Renamed some scripts; continued working on conversion-generalization
</commit_message>
<xml_diff>
--- a/Data/EC0206 Data Sources for DAC v2.xlsx
+++ b/Data/EC0206 Data Sources for DAC v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semarten\OneDrive for Business\Manuscripts\ECHO CEI Paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semarten\OneDrive for Business\Research\Creating_CE_Index\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>